<commit_message>
Feature(Tais): Modificando as telas de login e recuperação de senha para as novas cores padrões.
</commit_message>
<xml_diff>
--- a/Documentos/PBC - Cycle.xlsx
+++ b/Documentos/PBC - Cycle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://etecspgov-my.sharepoint.com/personal/tais_souza59_etec_sp_gov_br/Documents/Documentos/1 - BandTec/2ADSB/3 - Pesquisa e Inovação/cycle/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="254" documentId="8_{6279E8E0-1AA0-4C5F-9762-2C8B015BD0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2674C743-A60A-444E-ACE6-2719BB720CD4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBC" sheetId="15" r:id="rId1"/>
@@ -858,27 +858,27 @@
     </xf>
   </cellXfs>
   <cellStyles count="22">
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="21" builtinId="8"/>
+    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="48">
@@ -1976,8 +1976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.1" customHeight="1"/>
@@ -2758,7 +2758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>